<commit_message>
Delphi library and samples improved
</commit_message>
<xml_diff>
--- a/Samples/Delphi/VCL/Format/Format.xlsx
+++ b/Samples/Delphi/VCL/Format/Format.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t>Context</t>
   </si>
@@ -35,7 +35,7 @@
     <t>Hebrew</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TFORM1.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.Caption</t>
   </si>
   <si>
     <t>Sample</t>
@@ -50,7 +50,7 @@
     <t>Steekproef</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TFORM1.FirstNameLabel.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.FirstNameLabel.Caption</t>
   </si>
   <si>
     <t>&amp;First name:</t>
@@ -65,7 +65,7 @@
     <t>&amp;Voornaam:</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TFORM1.CountLabel.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.CountLabel.Caption</t>
   </si>
   <si>
     <t>&amp;Count:</t>
@@ -80,7 +80,7 @@
     <t>&amp;Telling:</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TFORM1.SecondNameLabel.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.SecondNameLabel.Caption</t>
   </si>
   <si>
     <t>&amp;Second name:</t>
@@ -95,7 +95,13 @@
     <t>&amp;Secondenaam:</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TFORM1.LanguageButton.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.CountEdit.Text</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>Win32\Release\Format.exe.RCData.TFORM1.LanguageButton.Caption</t>
   </si>
   <si>
     <t>&amp;Language...</t>
@@ -110,7 +116,7 @@
     <t>&amp;Taal...</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TNTLANGUAGEDIALOG.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TNTLANGUAGEDIALOG.Caption</t>
   </si>
   <si>
     <t>Select Language</t>
@@ -125,13 +131,13 @@
     <t>Selecteer Taal</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TNTLANGUAGEDIALOG.OkButton.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TNTLANGUAGEDIALOG.OkButton.Caption</t>
   </si>
   <si>
     <t>OK</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.RCData.TNTLANGUAGEDIALOG.CancelButton.Caption</t>
+    <t>Win32\Release\Format.exe.RCData.TNTLANGUAGEDIALOG.CancelButton.Caption</t>
   </si>
   <si>
     <t>Cancel</t>
@@ -146,85 +152,85 @@
     <t>Annuleren</t>
   </si>
   <si>
-    <t>Win32\\Release\\Format.exe.String.Unit1.SHello</t>
-  </si>
-  <si>
-    <t>Hello %s!</t>
-  </si>
-  <si>
-    <t>Moi %s!</t>
-  </si>
-  <si>
-    <t>Hallo %s!</t>
-  </si>
-  <si>
-    <t>Win32\\Release\\Format.exe.String.Unit1.SHello2</t>
-  </si>
-  <si>
-    <t>Hello %s and %s!</t>
-  </si>
-  <si>
-    <t>Moi %s ja %s!</t>
-  </si>
-  <si>
-    <t>Moi %1:s ja %0:s!</t>
-  </si>
-  <si>
-    <t>Hallo %s und %s!</t>
-  </si>
-  <si>
-    <t>Hallo %s en %s!</t>
-  </si>
-  <si>
-    <t>שלום %s %s!</t>
-  </si>
-  <si>
-    <t>Win32\\Release\\Format.exe.String.Unit1.SCount</t>
-  </si>
-  <si>
-    <t>%s has %d cars</t>
-  </si>
-  <si>
-    <t>%s:lla on %d autoa</t>
-  </si>
-  <si>
-    <t>%s hat %d Autos</t>
-  </si>
-  <si>
-    <t>%s heeft %d auto's</t>
-  </si>
-  <si>
-    <t>Win32\\Release\\Format.exe.String.Unit1.SCount2</t>
-  </si>
-  <si>
-    <t>%d cars will pick up %s and %s</t>
-  </si>
-  <si>
-    <t>%d autoa hakee %s:in ja %s:in</t>
-  </si>
-  <si>
-    <t>Autos nehmen %1:s und %2:s auf.</t>
-  </si>
-  <si>
-    <t>Auto's zullen %d ophalen %s en %s.</t>
-  </si>
-  <si>
-    <t>%d מכוניות יאספו %s ו-%s</t>
-  </si>
-  <si>
-    <t>Win32\\Release\\Format.exe.String.Unit1.SDouble</t>
-  </si>
-  <si>
-    <t>%0:s swims and %0:s skis</t>
-  </si>
-  <si>
-    <t>%0:s ui ja %0:s hiihtää</t>
+    <t>Win32\Release\Format.exe.String.Unit1.SHello</t>
+  </si>
+  <si>
+    <t>Hello {0}!</t>
+  </si>
+  <si>
+    <t>Moi {0}!</t>
+  </si>
+  <si>
+    <t>Hallo {0}!</t>
+  </si>
+  <si>
+    <t>Win32\Release\Format.exe.String.Unit1.SHello2</t>
+  </si>
+  <si>
+    <t>Hello {0} and {1}!</t>
+  </si>
+  <si>
+    <t>Moi {0} ja {1}!</t>
+  </si>
+  <si>
+    <t>Moi {1} ja {0}!</t>
+  </si>
+  <si>
+    <t>Hallo {0} und {1}!</t>
+  </si>
+  <si>
+    <t>Hallo {0} en {1}!</t>
+  </si>
+  <si>
+    <t>שלום {0} {1}!</t>
+  </si>
+  <si>
+    <t>Win32\Release\Format.exe.String.Unit1.SCount</t>
+  </si>
+  <si>
+    <t>{0} has {1} cars</t>
+  </si>
+  <si>
+    <t>{0}:lla on {1} autoa</t>
+  </si>
+  <si>
+    <t>{0} hat {1} Autos</t>
+  </si>
+  <si>
+    <t>{0} heeft {1} auto's</t>
+  </si>
+  <si>
+    <t>Win32\Release\Format.exe.String.Unit1.SCount2</t>
+  </si>
+  <si>
+    <t>{0} cars will pick up {1} and {2}</t>
+  </si>
+  <si>
+    <t>{0} autoa hakee {1}:in ja {2}:in</t>
+  </si>
+  <si>
+    <t>Autos nehmen {1} und {2} auf.</t>
+  </si>
+  <si>
+    <t>Auto's zullen {0} ophalen {1} en {2}.</t>
+  </si>
+  <si>
+    <t>{0} מכוניות יאספו {1} ו-{2}</t>
+  </si>
+  <si>
+    <t>Win32\Release\Format.exe.String.Unit1.SDouble</t>
+  </si>
+  <si>
+    <t>{0} swims and {0} skis</t>
+  </si>
+  <si>
+    <t>{0} ui ja {0} hiihtää</t>
   </si>
   <si>
     <t>Schwimmen und Skier</t>
   </si>
   <si>
-    <t>%0:s Zwemmen en %0:s ski's</t>
+    <t>{0} Zwemmen en {0} ski's</t>
   </si>
 </sst>
 </file>
@@ -526,7 +532,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:A1"/>
@@ -644,50 +650,44 @@
       <c r="B6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="C6" s="2"/>
       <c r="D6" s="2"/>
-      <c r="E6" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
       <c r="G6" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="7">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G7" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="8">
       <c r="A8" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>38</v>
@@ -702,119 +702,138 @@
         <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="G9" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="10">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G10" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="11">
       <c r="A11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>52</v>
-      </c>
       <c r="F11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>54</v>
-      </c>
+        <v>49</v>
+      </c>
+      <c r="G11" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="12">
       <c r="A12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="13">
       <c r="A13" s="2" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="G13" s="2"/>
     </row>
     <row ht="12.75" customHeight="1" r="14">
       <c r="A14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="2" t="s">
+    </row>
+    <row ht="12.75" customHeight="1" r="15">
+      <c r="A15" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="2"/>
+      <c r="D15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.78740157480315" right="0.78740157480315" top="0.78740157480315" bottom="0.78740157480315" header="0.393700787401575" footer="0.393700787401575"/>

</xml_diff>

<commit_message>
Composite string pattern changes
</commit_message>
<xml_diff>
--- a/Samples/Delphi/VCL/Format/Format.xlsx
+++ b/Samples/Delphi/VCL/Format/Format.xlsx
@@ -155,82 +155,82 @@
     <t>Win32\Release\Format.exe.String.Unit1.SHello</t>
   </si>
   <si>
-    <t>Hello {0}!</t>
-  </si>
-  <si>
-    <t>Moi {0}!</t>
-  </si>
-  <si>
-    <t>Hallo {0}!</t>
+    <t>Hello %s!</t>
+  </si>
+  <si>
+    <t>Moi %s!</t>
+  </si>
+  <si>
+    <t>Hallo %s!</t>
   </si>
   <si>
     <t>Win32\Release\Format.exe.String.Unit1.SHello2</t>
   </si>
   <si>
-    <t>Hello {0} and {1}!</t>
-  </si>
-  <si>
-    <t>Moi {0} ja {1}!</t>
-  </si>
-  <si>
-    <t>Moi {1} ja {0}!</t>
-  </si>
-  <si>
-    <t>Hallo {0} und {1}!</t>
-  </si>
-  <si>
-    <t>Hallo {0} en {1}!</t>
-  </si>
-  <si>
-    <t>שלום {0} {1}!</t>
+    <t>Hello %s and %s!</t>
+  </si>
+  <si>
+    <t>Moi %s ja %s!</t>
+  </si>
+  <si>
+    <t>Moi %1:s ja %0:s!</t>
+  </si>
+  <si>
+    <t>Hallo %s und %s!</t>
+  </si>
+  <si>
+    <t>Hallo %s en %s!</t>
+  </si>
+  <si>
+    <t>שלום %s %s!</t>
   </si>
   <si>
     <t>Win32\Release\Format.exe.String.Unit1.SCount</t>
   </si>
   <si>
-    <t>{0} has {1} cars</t>
-  </si>
-  <si>
-    <t>{0}:lla on {1} autoa</t>
-  </si>
-  <si>
-    <t>{0} hat {1} Autos</t>
-  </si>
-  <si>
-    <t>{0} heeft {1} auto's</t>
+    <t>%s has %d cars</t>
+  </si>
+  <si>
+    <t>%s:lla on %d autoa</t>
+  </si>
+  <si>
+    <t>%s hat %d Autos</t>
+  </si>
+  <si>
+    <t>%s heeft %d auto's</t>
   </si>
   <si>
     <t>Win32\Release\Format.exe.String.Unit1.SCount2</t>
   </si>
   <si>
-    <t>{0} cars will pick up {1} and {2}</t>
-  </si>
-  <si>
-    <t>{0} autoa hakee {1}:in ja {2}:in</t>
-  </si>
-  <si>
-    <t>Autos nehmen {1} und {2} auf.</t>
-  </si>
-  <si>
-    <t>Auto's zullen {0} ophalen {1} en {2}.</t>
-  </si>
-  <si>
-    <t>{0} מכוניות יאספו {1} ו-{2}</t>
+    <t>%d cars will pick up %s and %s</t>
+  </si>
+  <si>
+    <t>%d autoa hakee %s:in ja %s:in</t>
+  </si>
+  <si>
+    <t>Autos nehmen %1:s und %2:s auf.</t>
+  </si>
+  <si>
+    <t>Auto's zullen %d ophalen %s en %s.</t>
+  </si>
+  <si>
+    <t>%d מכוניות יאספו %s ו-%s</t>
   </si>
   <si>
     <t>Win32\Release\Format.exe.String.Unit1.SDouble</t>
   </si>
   <si>
-    <t>{0} swims and {0} skis</t>
-  </si>
-  <si>
-    <t>{0} ui ja {0} hiihtää</t>
+    <t>%0:s swims and %0:s skis</t>
+  </si>
+  <si>
+    <t>%0:s ui ja %0:s hiihtää</t>
   </si>
   <si>
     <t>Schwimmen und Skier</t>
   </si>
   <si>
-    <t>{0} Zwemmen en {0} ski's</t>
+    <t>%0:s Zwemmen en %0:s ski's</t>
   </si>
 </sst>
 </file>

</xml_diff>